<commit_message>
AAAAAAAAAAAAAAAAAAAA (Integrar los slides y el bloque con info)
</commit_message>
<xml_diff>
--- a/UrMaps_2_fase/descripciones_edificios.xlsx
+++ b/UrMaps_2_fase/descripciones_edificios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamour\Documents\GitHub\URMaps\URMaps\UrMaps_2_fase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e0575944bb8bd34/Documentos/GitHub/URMaps/UrMaps_2_fase/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA411B-B060-4337-8C7A-FB60BF5D1155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{38BFE892-4AFB-4984-BEC6-F26C714C6496}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{38BFE892-4AFB-4984-BEC6-F26C714C6496}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -262,18 +262,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -327,17 +321,17 @@
     <tableColumn id="3" xr3:uid="{67BC8874-90A2-4AAE-82ED-1E000ACD9EA5}" name="edif_fr" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{F07288BF-FB04-4967-B236-3F13177CF786}" name="desc_es" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{6F9B01DF-F617-44A5-9FB0-5D28F68F64AD}" name="desc_en" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{0F93CA16-93AE-4C57-8547-E347DF680BC1}" name="desc_fr" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{2C56FE3C-BBD1-4EEB-BC92-1C9F77CD78E6}" name="imagen" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{0F93CA16-93AE-4C57-8547-E347DF680BC1}" name="desc_fr" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2C56FE3C-BBD1-4EEB-BC92-1C9F77CD78E6}" name="imagen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -375,7 +369,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -481,7 +475,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -623,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,7 +631,7 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -647,18 +641,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1E28D0-1DF2-4337-A474-C551966BAA4F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="1" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="6" width="45.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -681,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -702,8 +696,8 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -723,14 +717,14 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -744,7 +738,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -765,7 +759,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -786,7 +780,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -796,7 +790,7 @@
       <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -807,7 +801,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -828,7 +822,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -849,7 +843,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -870,7 +864,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -893,8 +887,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>